<commit_message>
Update with Linz AG Data
TODO: add CO2 Cost
</commit_message>
<xml_diff>
--- a/app/modules/common/FEAT/F16/linz_ag/scenarios-mapper.xlsx
+++ b/app/modules/common/FEAT/F16/linz_ag/scenarios-mapper.xlsx
@@ -15,12 +15,12 @@
     <sheet name="scenarios" sheetId="6" r:id="rId1"/>
     <sheet name="sub-scenarios" sheetId="7" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
   <si>
     <t>name</t>
   </si>
@@ -28,31 +28,25 @@
     <t>file</t>
   </si>
   <si>
-    <t>Base Szenario</t>
-  </si>
-  <si>
-    <t>Szenario No Nuc Low C02</t>
-  </si>
-  <si>
-    <t>scenario_lzb</t>
-  </si>
-  <si>
-    <t>scenario_lzn</t>
-  </si>
-  <si>
-    <t>Current Price Scenario</t>
-  </si>
-  <si>
-    <t>Moderae Price Scenario</t>
-  </si>
-  <si>
-    <t>High Price Scenario</t>
-  </si>
-  <si>
-    <t>Low Price Scenario</t>
-  </si>
-  <si>
     <t>Prefix</t>
+  </si>
+  <si>
+    <t>Portfolio Status Quo</t>
+  </si>
+  <si>
+    <t>Scenario Hoch</t>
+  </si>
+  <si>
+    <t>Szenario Niedrig</t>
+  </si>
+  <si>
+    <t>Szenario Moderat</t>
+  </si>
+  <si>
+    <t>Szenario Quo</t>
+  </si>
+  <si>
+    <t>portfolio_quo</t>
   </si>
 </sst>
 </file>
@@ -463,10 +457,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -488,21 +482,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -515,7 +498,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -526,7 +509,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B1" s="2" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>0</v>
@@ -540,7 +523,7 @@
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -551,7 +534,7 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -562,7 +545,7 @@
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -573,7 +556,7 @@
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>